<commit_message>
Updated medicare for 2015-16
</commit_message>
<xml_diff>
--- a/data/medicare-tables.xlsx
+++ b/data/medicare-tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh\Documents\GitHub\grattan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romanesd\Documents\GitHub\rgrattan\grattan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="families" sheetId="3" r:id="rId2"/>
     <sheet name="SourceURL" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>fy_year</t>
   </si>
@@ -83,17 +83,20 @@
   </si>
   <si>
     <t>taper</t>
+  </si>
+  <si>
+    <t>2015-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,9 +137,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -231,6 +234,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -266,6 +286,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +493,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -479,7 +516,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -502,53 +539,53 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>32279</v>
+        <v>20896</v>
       </c>
       <c r="E4" s="1">
-        <v>37975</v>
+        <v>26121</v>
       </c>
       <c r="F4" s="3">
         <v>0.1</v>
       </c>
-      <c r="G4">
-        <v>1.4999999999999999E-2</v>
+      <c r="G4" s="2">
+        <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>20542</v>
+        <v>33044</v>
       </c>
       <c r="E5" s="1">
-        <v>24167</v>
+        <v>41306</v>
       </c>
       <c r="F5" s="3">
         <v>0.1</v>
       </c>
-      <c r="G5">
-        <v>1.4999999999999999E-2</v>
+      <c r="G5" s="2">
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -571,7 +608,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -594,19 +631,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>19404</v>
+        <v>32279</v>
       </c>
       <c r="E8" s="1">
-        <v>22828</v>
+        <v>37975</v>
       </c>
       <c r="F8" s="3">
         <v>0.1</v>
@@ -617,19 +654,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>30685</v>
+        <v>20542</v>
       </c>
       <c r="E9" s="1">
-        <v>36100</v>
+        <v>24167</v>
       </c>
       <c r="F9" s="3">
         <v>0.1</v>
@@ -646,13 +683,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>30452</v>
+        <v>19404</v>
       </c>
       <c r="E10" s="1">
-        <v>35824</v>
+        <v>22828</v>
       </c>
       <c r="F10" s="3">
         <v>0.1</v>
@@ -663,19 +700,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>18839</v>
+        <v>30685</v>
       </c>
       <c r="E11" s="1">
-        <v>22163</v>
+        <v>36100</v>
       </c>
       <c r="F11" s="3">
         <v>0.1</v>
@@ -686,19 +723,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>30685</v>
+        <v>30452</v>
       </c>
       <c r="E12" s="1">
-        <v>36100</v>
+        <v>35824</v>
       </c>
       <c r="F12" s="3">
         <v>0.1</v>
@@ -718,10 +755,10 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>30439</v>
+        <v>18839</v>
       </c>
       <c r="E13" s="1">
-        <v>35810</v>
+        <v>22163</v>
       </c>
       <c r="F13" s="3">
         <v>0.1</v>
@@ -732,19 +769,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
-        <v>18488</v>
+        <v>30685</v>
       </c>
       <c r="E14" s="1">
-        <v>21750</v>
+        <v>36100</v>
       </c>
       <c r="F14" s="3">
         <v>0.1</v>
@@ -755,19 +792,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>29867</v>
+        <v>30439</v>
       </c>
       <c r="E15" s="1">
-        <v>35137</v>
+        <v>35810</v>
       </c>
       <c r="F15" s="3">
         <v>0.1</v>
@@ -784,13 +821,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>27697</v>
+        <v>18488</v>
       </c>
       <c r="E16" s="1">
-        <v>32584</v>
+        <v>21750</v>
       </c>
       <c r="F16" s="3">
         <v>0.1</v>
@@ -801,19 +838,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>17794</v>
+        <v>29867</v>
       </c>
       <c r="E17" s="1">
-        <v>20934</v>
+        <v>35137</v>
       </c>
       <c r="F17" s="3">
         <v>0.1</v>
@@ -824,19 +861,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>28867</v>
+        <v>27697</v>
       </c>
       <c r="E18" s="1">
-        <v>33961</v>
+        <v>32584</v>
       </c>
       <c r="F18" s="3">
         <v>0.1</v>
@@ -853,13 +890,13 @@
         <v>0</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>25299</v>
+        <v>17794</v>
       </c>
       <c r="E19" s="1">
-        <v>29763</v>
+        <v>20934</v>
       </c>
       <c r="F19" s="3">
         <v>0.1</v>
@@ -870,19 +907,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>17309</v>
+        <v>28867</v>
       </c>
       <c r="E20" s="1">
-        <v>20363</v>
+        <v>33961</v>
       </c>
       <c r="F20" s="3">
         <v>0.1</v>
@@ -893,19 +930,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>25867</v>
+        <v>25299</v>
       </c>
       <c r="E21" s="1">
-        <v>30431</v>
+        <v>29763</v>
       </c>
       <c r="F21" s="3">
         <v>0.1</v>
@@ -922,13 +959,13 @@
         <v>0</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>22922</v>
+        <v>17309</v>
       </c>
       <c r="E22" s="1">
-        <v>26967</v>
+        <v>20363</v>
       </c>
       <c r="F22" s="3">
         <v>0.1</v>
@@ -939,19 +976,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>16740</v>
+        <v>25867</v>
       </c>
       <c r="E23" s="1">
-        <v>19694</v>
+        <v>30431</v>
       </c>
       <c r="F23" s="3">
         <v>0.1</v>
@@ -962,19 +999,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>24867</v>
+        <v>22922</v>
       </c>
       <c r="E24" s="1">
-        <v>29255</v>
+        <v>26967</v>
       </c>
       <c r="F24" s="3">
         <v>0.1</v>
@@ -991,18 +1028,64 @@
         <v>0</v>
       </c>
       <c r="C25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1">
+        <v>16740</v>
+      </c>
+      <c r="E25" s="1">
+        <v>19694</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>24867</v>
+      </c>
+      <c r="E26" s="1">
+        <v>29255</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G26">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
         <v>21637</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E27" s="1">
         <v>25455</v>
       </c>
-      <c r="F25" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G25">
+      <c r="F27" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G27">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>

</xml_diff>